<commit_message>
Nuevo intento de clase de medición de tiempos
</commit_message>
<xml_diff>
--- a/src/main/java/algestudiante/p6/P6_UO277876.xlsx
+++ b/src/main/java/algestudiante/p6/P6_UO277876.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\infer\git\alg_AunonAndreaUO277876\src\main\java\algestudiante\p6\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62D6C35A-D7C7-41A3-920C-27CFE6AEAC61}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{094EBE03-B438-4932-B3D8-FAB386ED5909}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{760BF4A0-4F21-48FC-9449-0A68ABD67C67}"/>
+    <workbookView xWindow="11796" yWindow="720" windowWidth="10764" windowHeight="9480" xr2:uid="{760BF4A0-4F21-48FC-9449-0A68ABD67C67}"/>
   </bookViews>
   <sheets>
     <sheet name="Backtracking" sheetId="5" r:id="rId1"/>
@@ -57,13 +57,13 @@
     <t>Complejidad:</t>
   </si>
   <si>
-    <t>t(Prog. Dinámica)</t>
-  </si>
-  <si>
     <t>nVeces (Prog. Dinámica)</t>
   </si>
   <si>
     <t>O(n!)</t>
+  </si>
+  <si>
+    <t>t(backtracking)</t>
   </si>
 </sst>
 </file>
@@ -388,7 +388,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>t(Prog. Dinámica)</c:v>
+                  <c:v>t(backtracking)</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1564,7 +1564,7 @@
   <dimension ref="A2:I12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1583,10 +1583,10 @@
         <v>4</v>
       </c>
       <c r="B2" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" s="11" t="s">
         <v>7</v>
-      </c>
-      <c r="C2" s="11" t="s">
-        <v>8</v>
       </c>
       <c r="F2" s="4" t="s">
         <v>1</v>
@@ -1689,7 +1689,7 @@
         <v>6</v>
       </c>
       <c r="B9" s="16" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C9" s="15"/>
       <c r="I9" s="13">

</xml_diff>

<commit_message>
Creación del constructor n
</commit_message>
<xml_diff>
--- a/src/main/java/algestudiante/p6/P6_UO277876.xlsx
+++ b/src/main/java/algestudiante/p6/P6_UO277876.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\infer\git\alg_AunonAndreaUO277876\src\main\java\algestudiante\p6\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9659E0B5-3C18-4F4E-B721-696079C2332F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D7D7696-F9B5-4FC0-BB41-3AF12DE9F042}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11796" yWindow="720" windowWidth="10764" windowHeight="9480" xr2:uid="{760BF4A0-4F21-48FC-9449-0A68ABD67C67}"/>
+    <workbookView xWindow="12144" yWindow="1068" windowWidth="10764" windowHeight="9480" xr2:uid="{760BF4A0-4F21-48FC-9449-0A68ABD67C67}"/>
   </bookViews>
   <sheets>
     <sheet name="Backtracking" sheetId="5" r:id="rId1"/>
@@ -423,19 +423,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>100</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>200</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>400</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>800</c:v>
+                  <c:v>25</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1600</c:v>
+                  <c:v>30</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>3200</c:v>
@@ -450,19 +450,19 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>25.01</c:v>
+                  <c:v>4.09</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2.4569999999999999</c:v>
+                  <c:v>3.37</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2.4159999999999999</c:v>
+                  <c:v>2.69</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>2.69</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>2.98</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1560,7 +1560,7 @@
   <dimension ref="A2:I23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1594,11 +1594,11 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" s="15">
-        <v>100</v>
+        <v>5</v>
       </c>
       <c r="B3" s="17">
-        <f>2501/I10</f>
-        <v>25.01</v>
+        <f>409/I10</f>
+        <v>4.09</v>
       </c>
       <c r="C3" s="12" t="s">
         <v>9</v>
@@ -1613,11 +1613,11 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" s="15">
-        <v>200</v>
+        <v>10</v>
       </c>
       <c r="B4" s="17">
-        <f>2457/I9</f>
-        <v>2.4569999999999999</v>
+        <f>337/I10</f>
+        <v>3.37</v>
       </c>
       <c r="C4" s="12"/>
       <c r="F4" s="8" t="s">
@@ -1630,11 +1630,11 @@
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" s="15">
-        <v>400</v>
+        <v>15</v>
       </c>
       <c r="B5" s="17">
-        <f>2416/I9</f>
-        <v>2.4159999999999999</v>
+        <f>269/I10</f>
+        <v>2.69</v>
       </c>
       <c r="C5" s="12"/>
       <c r="I5" s="2">
@@ -1643,11 +1643,11 @@
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" s="15">
-        <v>800</v>
+        <v>25</v>
       </c>
       <c r="B6" s="17">
-        <f>B10/I9</f>
-        <v>0</v>
+        <f>269/I10</f>
+        <v>2.69</v>
       </c>
       <c r="C6" s="12"/>
       <c r="I6" s="2">
@@ -1656,11 +1656,11 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" s="15">
-        <v>1600</v>
-      </c>
-      <c r="B7" s="17" t="e">
-        <f>123775/N9</f>
-        <v>#DIV/0!</v>
+        <v>30</v>
+      </c>
+      <c r="B7" s="17">
+        <f>298/I10</f>
+        <v>2.98</v>
       </c>
       <c r="C7" s="12"/>
       <c r="I7" s="3">

</xml_diff>